<commit_message>
first commit from venv before MFA solving problem
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -395,40 +395,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1">
-        <v>0</v>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>